<commit_message>
change select brand logic
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/search.xlsx
+++ b/src/test/resources/xls/search.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Документ был экспортирован из Numbers. Каждая таблица была конвертирована в рабочий лист Excel. Все другие объекты на листах Numbers были помещены на отдельные рабочие листы. Имейте в виду, что расчеты формул могут отличаться от расчетов в Excel.</t>
   </si>
@@ -27,10 +27,38 @@
     <t>Название рабочего листа Excel</t>
   </si>
   <si>
+    <t>Обзор экспорта</t>
+  </si>
+  <si>
+    <t>Tаблица 1</t>
+  </si>
+  <si>
     <t>newsGSM</t>
   </si>
   <si>
-    <t>Tаблица 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>newsGSM</t>
+    </r>
+  </si>
+  <si>
+    <t>phoneFinder</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>phoneFinder</t>
+    </r>
   </si>
   <si>
     <t>Execute</t>
@@ -60,9 +88,6 @@
     <t>cat</t>
   </si>
   <si>
-    <t>phoneFinder</t>
-  </si>
-  <si>
     <t>brand</t>
   </si>
   <si>
@@ -70,6 +95,9 @@
   </si>
   <si>
     <t>Xiaomi</t>
+  </si>
+  <si>
+    <t>Acer</t>
   </si>
 </sst>
 </file>
@@ -109,12 +137,12 @@
     <font>
       <b val="1"/>
       <sz val="10"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
       <name val="Helvetica Neue Medium"/>
     </font>
     <font>
@@ -145,17 +173,104 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -175,13 +290,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="15"/>
@@ -190,7 +320,52 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
       </left>
       <right style="thin">
         <color indexed="15"/>
@@ -199,7 +374,7 @@
         <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
@@ -208,73 +383,13 @@
         <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
         <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
         <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
@@ -284,7 +399,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -306,67 +421,136 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -389,6 +573,7 @@
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff323232"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffa5a5a5"/>
@@ -1454,73 +1639,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.6719" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.6719" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.7" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="14.7" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="20"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Обзор экспорта'!R1C1" tooltip="" display="Обзор экспорта"/>
     <hyperlink ref="D10" location="'newsGSM'!R1C1" tooltip="" display="newsGSM"/>
     <hyperlink ref="D12" location="'phoneFinder'!R1C1" tooltip="" display="phoneFinder"/>
+    <hyperlink ref="D12" location="'newsGSM'!R1C1" tooltip="" display="newsGSM"/>
+    <hyperlink ref="D14" location="'phoneFinder'!R1C1" tooltip="" display="phoneFinder"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1532,235 +1806,235 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.6719" style="6" customWidth="1"/>
-    <col min="2" max="7" width="16.3516" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.6719" style="25" customWidth="1"/>
+    <col min="2" max="7" width="16.3516" style="25" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.65" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="A1" t="s" s="26">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
+      <c r="A2" t="s" s="28">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="29">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s" s="29">
+        <v>15</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" ht="20.3" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
+      <c r="A3" t="s" s="28">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
     </row>
     <row r="4" ht="19.95" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" ht="19.95" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" ht="19.95" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" ht="19.95" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" ht="19.95" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" ht="19.95" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" ht="19.95" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" ht="19.95" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" ht="19.95" customHeight="1">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" ht="19.95" customHeight="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" ht="19.95" customHeight="1">
-      <c r="A14" s="16"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" ht="19.95" customHeight="1">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" ht="19.95" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" ht="19.95" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" ht="19.95" customHeight="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" ht="19.95" customHeight="1">
-      <c r="A19" s="16"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" ht="19.95" customHeight="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" ht="19.95" customHeight="1">
-      <c r="A21" s="16"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" ht="19.95" customHeight="1">
-      <c r="A22" s="16"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" ht="20.2" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -1778,101 +2052,107 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="17" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="17" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="36" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="18">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="18">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="18">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s" s="18">
+      <c r="A1" t="s" s="37">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s" s="37">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s" s="37">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s" s="37">
+        <v>20</v>
+      </c>
+      <c r="E1" s="38"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="39">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="40">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s" s="41">
+        <v>21</v>
+      </c>
+      <c r="D2" s="42">
+        <v>276</v>
+      </c>
+      <c r="E2" s="43"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="44">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s" s="45">
         <v>17</v>
       </c>
-      <c r="E1" s="19"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="20">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s" s="21">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s" s="22">
-        <v>18</v>
-      </c>
-      <c r="D2" s="23">
-        <v>276</v>
-      </c>
-      <c r="E2" s="24"/>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" t="s" s="46">
+        <v>22</v>
+      </c>
+      <c r="D3" s="47">
+        <v>69</v>
+      </c>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>